<commit_message>
Latest Testrigs reports updated
</commit_message>
<xml_diff>
--- a/minio-report-tracker/xlxs/cellbox21.xlsx
+++ b/minio-report-tracker/xlxs/cellbox21.xlsx
@@ -722,7 +722,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -774,7 +774,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -785,13 +785,13 @@
         <v>512</v>
       </c>
       <c r="D2" t="n">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -813,13 +813,13 @@
         <v>512</v>
       </c>
       <c r="D3" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" t="n">
         <v>4</v>
@@ -830,27 +830,27 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45844</v>
+        <v>45845</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>auth</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>512</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>493</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -869,13 +869,13 @@
         <v>410</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="E5" t="n">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
         <v>84</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -897,13 +897,13 @@
         <v>410</v>
       </c>
       <c r="D6" t="n">
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="F6" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
         <v>84</v>
@@ -914,27 +914,27 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>945</v>
+        <v>410</v>
       </c>
       <c r="D7" t="n">
-        <v>920</v>
+        <v>322</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G7" t="n">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -974,14 +974,14 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C9" t="n">
         <v>945</v>
       </c>
       <c r="D9" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -1002,14 +1002,14 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C10" t="n">
         <v>945</v>
       </c>
       <c r="D10" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
@@ -1018,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1026,18 +1026,18 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C11" t="n">
         <v>945</v>
       </c>
       <c r="D11" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
@@ -1046,7 +1046,7 @@
         <v>10</v>
       </c>
       <c r="G11" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -1054,18 +1054,18 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C12" t="n">
         <v>945</v>
       </c>
       <c r="D12" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
@@ -1074,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="G12" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
         <v>0</v>
@@ -1082,18 +1082,18 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>945</v>
       </c>
       <c r="D13" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1102,7 +1102,7 @@
         <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1110,11 +1110,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1142,7 +1142,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1194,11 +1194,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1222,11 +1222,11 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1250,58 +1250,58 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D19" t="n">
-        <v>332</v>
+        <v>920</v>
       </c>
       <c r="E19" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H19" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D20" t="n">
-        <v>497</v>
+        <v>920</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G20" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H20" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1310,23 +1310,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D21" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G21" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
@@ -1338,23 +1338,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D22" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G22" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H22" t="n">
         <v>0</v>
@@ -1362,27 +1362,27 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1126</v>
+        <v>945</v>
       </c>
       <c r="D23" t="n">
-        <v>1106</v>
+        <v>920</v>
       </c>
       <c r="E23" t="n">
         <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G23" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H23" t="n">
         <v>0</v>
@@ -1390,27 +1390,27 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1126</v>
+        <v>945</v>
       </c>
       <c r="D24" t="n">
-        <v>1117</v>
+        <v>920</v>
       </c>
       <c r="E24" t="n">
         <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1418,27 +1418,27 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>945</v>
       </c>
       <c r="D25" t="n">
-        <v>3</v>
+        <v>920</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G25" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H25" t="n">
         <v>0</v>
@@ -1446,29 +1446,337 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>509</v>
+      </c>
+      <c r="D26" t="n">
+        <v>332</v>
+      </c>
+      <c r="E26" t="n">
+        <v>134</v>
+      </c>
+      <c r="F26" t="n">
+        <v>31</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>509</v>
+      </c>
+      <c r="D27" t="n">
+        <v>332</v>
+      </c>
+      <c r="E27" t="n">
+        <v>134</v>
+      </c>
+      <c r="F27" t="n">
+        <v>31</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
         <v>45845</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>pms</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>509</v>
+      </c>
+      <c r="D28" t="n">
+        <v>497</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>288</v>
+      </c>
+      <c r="D29" t="n">
+        <v>280</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>2</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>288</v>
+      </c>
+      <c r="D30" t="n">
+        <v>280</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>6</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>288</v>
+      </c>
+      <c r="D31" t="n">
+        <v>280</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D32" t="n">
+        <v>880</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>234</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1106</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>20</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1117</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>9</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C35" t="n">
         <v>3</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D35" t="n">
         <v>2</v>
       </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
         <v>1</v>
       </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>3</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CSV and XLSX reports
</commit_message>
<xml_diff>
--- a/minio-report-tracker/xlxs/cellbox21.xlsx
+++ b/minio-report-tracker/xlxs/cellbox21.xlsx
@@ -723,7 +723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,7 +785,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -796,13 +796,13 @@
         <v>512</v>
       </c>
       <c r="D2" t="n">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="n">
         <v>4</v>
@@ -813,7 +813,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -824,13 +824,13 @@
         <v>512</v>
       </c>
       <c r="D3" t="n">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="n">
         <v>4</v>
@@ -841,7 +841,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -852,13 +852,13 @@
         <v>512</v>
       </c>
       <c r="D4" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" t="n">
         <v>4</v>
@@ -869,27 +869,27 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45844</v>
+        <v>45845</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>auth</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>512</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>493</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45843</v>
+        <v>45844</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -925,7 +925,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -936,13 +936,13 @@
         <v>410</v>
       </c>
       <c r="D7" t="n">
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="F7" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
         <v>84</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -964,13 +964,13 @@
         <v>410</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="E8" t="n">
-        <v>326</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" t="n">
         <v>84</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -992,13 +992,13 @@
         <v>410</v>
       </c>
       <c r="D9" t="n">
-        <v>322</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>326</v>
       </c>
       <c r="F9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>84</v>
@@ -1009,27 +1009,27 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45847</v>
+        <v>45845</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>masterdata-ara</t>
+          <t>idrepo</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>945</v>
+        <v>410</v>
       </c>
       <c r="D10" t="n">
-        <v>920</v>
+        <v>322</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G10" t="n">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45846</v>
+        <v>45848</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1093,18 +1093,18 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45847</v>
+        <v>45846</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C13" t="n">
         <v>945</v>
       </c>
       <c r="D13" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
@@ -1113,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H13" t="n">
         <v>0</v>
@@ -1121,18 +1121,18 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>masterdata-eng</t>
+          <t>masterdata-ara</t>
         </is>
       </c>
       <c r="C14" t="n">
         <v>945</v>
       </c>
       <c r="D14" t="n">
-        <v>935</v>
+        <v>920</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
@@ -1141,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H14" t="n">
         <v>0</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45845</v>
+        <v>45848</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1181,14 +1181,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C16" t="n">
         <v>945</v>
       </c>
       <c r="D16" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>10</v>
       </c>
       <c r="G16" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
@@ -1209,14 +1209,14 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C17" t="n">
         <v>945</v>
       </c>
       <c r="D17" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>10</v>
       </c>
       <c r="G17" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
         <v>0</v>
@@ -1237,14 +1237,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>masterdata-fra</t>
+          <t>masterdata-eng</t>
         </is>
       </c>
       <c r="C18" t="n">
         <v>945</v>
       </c>
       <c r="D18" t="n">
-        <v>920</v>
+        <v>935</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1253,7 +1253,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -1261,11 +1261,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1289,11 +1289,11 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1317,11 +1317,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>masterdata-hin</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1345,11 +1345,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>45847</v>
+        <v>45845</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-fra</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1373,11 +1373,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45846</v>
+        <v>45848</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1401,11 +1401,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>masterdata-kan</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1429,11 +1429,11 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45847</v>
+        <v>45846</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1457,11 +1457,11 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-hin</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1485,11 +1485,11 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>45845</v>
+        <v>45848</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>masterdata-tam</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1517,26 +1517,26 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D28" t="n">
-        <v>332</v>
+        <v>920</v>
       </c>
       <c r="E28" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H28" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1545,26 +1545,26 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D29" t="n">
-        <v>332</v>
+        <v>920</v>
       </c>
       <c r="E29" t="n">
-        <v>134</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H29" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1573,51 +1573,51 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>pms</t>
+          <t>masterdata-kan</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>509</v>
+        <v>945</v>
       </c>
       <c r="D30" t="n">
-        <v>497</v>
+        <v>920</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H30" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45847</v>
+        <v>45848</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D31" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G31" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H31" t="n">
         <v>0</v>
@@ -1625,27 +1625,27 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45846</v>
+        <v>45847</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D32" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E32" t="n">
         <v>0</v>
       </c>
       <c r="F32" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G32" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H32" t="n">
         <v>0</v>
@@ -1653,27 +1653,27 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>45845</v>
+        <v>45846</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>prereg</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>288</v>
+        <v>945</v>
       </c>
       <c r="D33" t="n">
-        <v>280</v>
+        <v>920</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G33" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -1681,27 +1681,27 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45847</v>
+        <v>45845</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>masterdata-tam</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1126</v>
+        <v>945</v>
       </c>
       <c r="D34" t="n">
-        <v>880</v>
+        <v>920</v>
       </c>
       <c r="E34" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H34" t="n">
         <v>0</v>
@@ -1709,102 +1709,102 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>45846</v>
+        <v>45848</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1126</v>
+        <v>509</v>
       </c>
       <c r="D35" t="n">
-        <v>1106</v>
+        <v>332</v>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F35" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="G35" t="n">
         <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>45845</v>
+        <v>45847</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>resident</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1126</v>
+        <v>509</v>
       </c>
       <c r="D36" t="n">
-        <v>1117</v>
+        <v>332</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F36" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="G36" t="n">
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>45847</v>
+        <v>45846</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>509</v>
       </c>
       <c r="D37" t="n">
-        <v>2</v>
+        <v>332</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>134</v>
       </c>
       <c r="F37" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>dsl</t>
+          <t>pms</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>509</v>
       </c>
       <c r="D38" t="n">
-        <v>3</v>
+        <v>497</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -1816,34 +1816,314 @@
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
+        <v>45848</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>288</v>
+      </c>
+      <c r="D39" t="n">
+        <v>280</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>6</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>288</v>
+      </c>
+      <c r="D40" t="n">
+        <v>280</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>288</v>
+      </c>
+      <c r="D41" t="n">
+        <v>280</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>6</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
         <v>45845</v>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>prereg</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>288</v>
+      </c>
+      <c r="D42" t="n">
+        <v>280</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>6</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>45848</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D43" t="n">
+        <v>874</v>
+      </c>
+      <c r="E43" t="n">
+        <v>12</v>
+      </c>
+      <c r="F43" t="n">
+        <v>240</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D44" t="n">
+        <v>880</v>
+      </c>
+      <c r="E44" t="n">
+        <v>12</v>
+      </c>
+      <c r="F44" t="n">
+        <v>234</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1106</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>20</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>resident</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1126</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1117</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" t="n">
+        <v>9</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45847</v>
+      </c>
+      <c r="B47" t="inlineStr">
         <is>
           <t>dsl</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="C47" t="n">
         <v>3</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D47" t="n">
         <v>2</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
         <v>1</v>
       </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>45846</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" t="n">
+        <v>3</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>45845</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>dsl</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>3</v>
+      </c>
+      <c r="D49" t="n">
+        <v>2</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>